<commit_message>
Crear Endpoint descargar archivos con un ZIP
</commit_message>
<xml_diff>
--- a/controllers/files/Acta Apoyo a la Inversion Plantilla.xlsx
+++ b/controllers/files/Acta Apoyo a la Inversion Plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Residencia\Archivos Para Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E68CD8-68F5-4ECE-A98B-AF3C27FD3573}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7893C6-048E-428F-88EB-FDC133956CA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="906" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -449,106 +449,100 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>35718</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>35723</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>205741</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>68975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>586741</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>54772</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="3 Imagen" descr="C:\Users\AMERICA\Desktop\LOGO.jpg">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA911EEC-B922-417A-B183-F15BB0604C8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="35718" y="35723"/>
-          <a:ext cx="1762125" cy="923924"/>
+          <a:off x="3985261" y="350915"/>
+          <a:ext cx="2857500" cy="557770"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>59533</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>35721</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>144781</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>36191</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>643098</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>35721</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>144781</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="4 Imagen" descr="C:\Users\AMERICA\Desktop\LOGO 2.jpg">
+        <xdr:cNvPr id="7" name="Imagen 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C72B2569-49F5-42AF-AEB8-C6D10B18B75C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="5031583" y="35721"/>
-          <a:ext cx="1688465" cy="895350"/>
+          <a:off x="144781" y="165731"/>
+          <a:ext cx="1424940" cy="977269"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -822,7 +816,7 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Backend Correciones 7 ene
</commit_message>
<xml_diff>
--- a/controllers/files/Acta Apoyo a la Inversion Plantilla.xlsx
+++ b/controllers/files/Acta Apoyo a la Inversion Plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Residencia\Archivos Para Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7893C6-048E-428F-88EB-FDC133956CA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74A4DA4-1C82-414E-BC10-254CC883C19D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="906" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1345,14 +1345,14 @@
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="13"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="A46" s="48"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="49"/>
       <c r="E46" s="49"/>
       <c r="F46" s="49"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="14"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="50"/>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -1412,7 +1412,7 @@
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="A45:H45"/>
-    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="A46:H46"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.26" top="0.3" bottom="0.3" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>